<commit_message>
Bug fix to EHPpUC
</commit_message>
<xml_diff>
--- a/InputData/hydgn/EHPpUC/Electrolyzer Hydrogen Production per Unit Capacity.xlsx
+++ b/InputData/hydgn/EHPpUC/Electrolyzer Hydrogen Production per Unit Capacity.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipD\InputData\hydgn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-texas\InputData\hydgn\EHPpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Source:</t>
   </si>
@@ -95,13 +95,22 @@
   </si>
   <si>
     <t>BTU H2 / MW (annual production)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The study they are citing uses 3 scenarios of Fuel Cell Electric Vehicle adoption. Then it calculates the amount of hydrogen needed to suppor those vehicles. Then it calculates the electrolyzer capacity needed to supply that hydrogen. </t>
+  </si>
+  <si>
+    <t>So, I think it's fair, using the EPS assumptions of 24/7/365 operation, that smallest electrolyzer you would need to produce 1.39e10 annual Btu would be 1 MW.</t>
+  </si>
+  <si>
+    <t>No reason to think this would be different for Texas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +130,38 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -153,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -166,6 +207,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -449,16 +506,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,47 +525,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="B4" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -521,24 +580,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="5" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.1328125" customWidth="1"/>
+    <col min="3" max="3" width="27.46484375" customWidth="1"/>
+    <col min="4" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
@@ -552,8 +619,18 @@
       <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -567,8 +644,18 @@
         <f>B3/C3</f>
         <v>264.14473684210526</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -579,11 +666,16 @@
         <v>608</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E5" si="0">B4/C4</f>
+        <f>B4/C4</f>
         <v>264.14473684210526</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -594,18 +686,35 @@
         <v>1140</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5" si="0">B5/C5</f>
         <v>264.14473684210526</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>23874</v>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.4">
+      <c r="A8" s="9">
+        <v>60920</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -614,29 +723,159 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="9" spans="1:15" ht="15.4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:15">
+      <c r="A12">
         <v>2204.62</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="C13" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <f>E3*A11*A8</f>
-        <v>13902755788.697367</v>
-      </c>
+      <c r="C14" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="6">
+        <f>E3*A12*A8</f>
+        <v>35476077852.368416</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="D16" s="14"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="4:9">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="4:9">
+      <c r="D18" s="14"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="4:9">
+      <c r="D19" s="14"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="4:9">
+      <c r="D20" s="14"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="4:9">
+      <c r="D21" s="14"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="4:9">
+      <c r="D22" s="14"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="4:9">
+      <c r="D23" s="14"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="4:9">
+      <c r="D24" s="14"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="4:9">
+      <c r="D25" s="14"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="4:9">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="4:9">
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="4:9">
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -653,14 +892,16 @@
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35">
       <c r="B1">
         <v>2017</v>
       </c>
@@ -764,145 +1005,145 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="C2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="D2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="E2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="F2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="G2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="H2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="I2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="J2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="K2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="L2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="M2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="N2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="O2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="P2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="Q2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="R2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="S2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="T2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="U2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="V2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="W2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="X2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="Y2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="Z2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AA2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AB2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AC2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AD2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AE2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AF2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AG2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AH2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
       <c r="AI2" s="6">
-        <f>Calculations!$A$14</f>
-        <v>13902755788.697367</v>
+        <f>Calculations!$A$15</f>
+        <v>35476077852.368416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>